<commit_message>
fixed format issue on product backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog/product backlog.xlsx
+++ b/Product_Backlog/product backlog.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johng\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{915AFCBE-AF4D-4D61-A427-772C8BBB8194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="300" windowWidth="15375" windowHeight="7875" xr2:uid="{67798CE7-5B20-4196-9FFE-C18CDE4CB71B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -218,7 +217,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,12 +259,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -267,6 +268,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,17 +590,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79B7B28-A6E3-47B6-8D9C-9D113E809992}">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.85546875" customWidth="1"/>
-    <col min="2" max="2" width="105.28515625" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="66.85546875" customWidth="1"/>
@@ -598,379 +608,438 @@
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="8">
         <v>43853</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="8">
         <v>43853</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="1">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="8">
         <v>43853</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="1">
+      <c r="F6" s="5"/>
+      <c r="G6" s="8">
         <v>43853</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>10</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="1">
+      <c r="F7" s="5"/>
+      <c r="G7" s="8">
         <v>43853</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>9</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G8" s="8">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="8">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8">
+        <v>43852</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
+      <c r="C11" s="5">
+        <v>7</v>
+      </c>
+      <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="G11" s="8">
+        <v>43852</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10">
+      <c r="C12" s="5">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
         <v>2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11">
+      <c r="G12" s="8">
+        <v>43852</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="8">
+        <v>43852</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="8">
+        <v>43852</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="8">
+        <v>43852</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5">
         <v>4</v>
       </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12">
+      <c r="E16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="8">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="5">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13">
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="8">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="F15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17">
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="8">
+        <v>43852</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="5">
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D19" s="5">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="1">
-        <v>43852</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="8">
         <v>43852</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>